<commit_message>
updated excel docs and comments
</commit_message>
<xml_diff>
--- a/excel_docs/starting_ex/example_start.xlsx
+++ b/excel_docs/starting_ex/example_start.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\highlight_excels\excel_docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/648742649a6f8c0c/Documents/GitHub/highlight_excels/excel_docs/starting_ex/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096A58D2-B3B4-46C4-8FD5-FEF1D275AC82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{096A58D2-B3B4-46C4-8FD5-FEF1D275AC82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30CC2A06-CC71-4CCD-B43B-8DEF2031EA61}"/>
   <bookViews>
-    <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8880" xr2:uid="{3C6329DF-4F8C-4069-8EEF-F5CC61BABC37}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3C6329DF-4F8C-4069-8EEF-F5CC61BABC37}"/>
   </bookViews>
   <sheets>
     <sheet name="books" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
   <si>
     <t>ratings (x/5)</t>
   </si>
@@ -124,12 +124,6 @@
     <t>014242417X</t>
   </si>
   <si>
-    <t>hhhhhhhhh</t>
-  </si>
-  <si>
-    <t>kjh;lkj;kl</t>
-  </si>
-  <si>
     <t>5</t>
   </si>
   <si>
@@ -139,13 +133,10 @@
     <t>3</t>
   </si>
   <si>
-    <t>ISBNs (kinda)</t>
-  </si>
-  <si>
     <t>books</t>
   </si>
   <si>
-    <t>baking pi</t>
+    <t>ISBNs</t>
   </si>
 </sst>
 </file>
@@ -523,8 +514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{404AE3F7-2DD2-4B91-A156-BCF8DD69F515}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -537,11 +528,11 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
@@ -570,7 +561,7 @@
         <v>439136350</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -584,7 +575,7 @@
         <v>60837020</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -598,7 +589,7 @@
         <v>808514571</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -612,7 +603,7 @@
         <v>28</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -626,7 +617,7 @@
         <v>142402516</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -640,7 +631,7 @@
         <v>525487085</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -654,7 +645,7 @@
         <v>385486804</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -668,7 +659,7 @@
         <v>1285159454</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -678,11 +669,11 @@
       <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>29</v>
+      <c r="C11" s="3">
+        <v>1285159454</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -692,11 +683,11 @@
       <c r="B12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="3">
+        <v>1285159454</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -710,7 +701,7 @@
         <v>980852233</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -724,7 +715,7 @@
         <v>343455345</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -738,7 +729,7 @@
         <v>654654</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -752,21 +743,12 @@
         <v>65465465</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="2">
-        <v>3.14</v>
-      </c>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C17" s="3">
-        <v>142402516</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>31</v>
+        <v>1285159454</v>
       </c>
     </row>
   </sheetData>

</xml_diff>